<commit_message>
updated the category file
</commit_message>
<xml_diff>
--- a/event_category.xlsx
+++ b/event_category.xlsx
@@ -10,14 +10,14 @@
     <sheet name="event_category" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">event_category!$A$1:$B$429</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">event_category!#REF!</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="454">
   <si>
     <t xml:space="preserve">Event </t>
   </si>
@@ -1322,13 +1322,70 @@
   </si>
   <si>
     <t>DUST / FOG</t>
+  </si>
+  <si>
+    <t>FLOOD/RAIN/WINDS</t>
+  </si>
+  <si>
+    <t>COOL AND WET</t>
+  </si>
+  <si>
+    <t>COLD AND WET CONDITIONS</t>
+  </si>
+  <si>
+    <t>EXCESSIVE WETNESS</t>
+  </si>
+  <si>
+    <t>SMALL STREAM FLOOD</t>
+  </si>
+  <si>
+    <t>HVY RAIN</t>
+  </si>
+  <si>
+    <t>HAIL 150</t>
+  </si>
+  <si>
+    <t>HAIL 075</t>
+  </si>
+  <si>
+    <t>HAIL 125</t>
+  </si>
+  <si>
+    <t>THUNDERSTORM WIND G60</t>
+  </si>
+  <si>
+    <t>THUNDERSTORM WINDS G60</t>
+  </si>
+  <si>
+    <t>HARD FREEZE</t>
+  </si>
+  <si>
+    <t>HAIL 200</t>
+  </si>
+  <si>
+    <t>THUNDERSTORM WIND.</t>
+  </si>
+  <si>
+    <t>TORNADOES</t>
+  </si>
+  <si>
+    <t>Unseasonable Cold</t>
+  </si>
+  <si>
+    <t>Early Frost</t>
+  </si>
+  <si>
+    <t>AGRICULTURAL FREEZE</t>
+  </si>
+  <si>
+    <t>UNSEASONAL RAIN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1360,6 +1417,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1387,12 +1450,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1694,10 +1760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B429"/>
+  <dimension ref="A1:B523"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5138,6 +5204,215 @@
         <v>416</v>
       </c>
     </row>
+    <row r="430" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A430" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="B430" s="4" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="431" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A431" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="B431" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="432" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A432" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="B432" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="433" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A433" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="B433" s="4" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="434" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A434" s="5" t="s">
+        <v>439</v>
+      </c>
+      <c r="B434" s="4" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="435" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A435" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="B435" s="4" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="436" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A436" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="B436" s="4" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="437" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A437" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="B437" s="4" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="438" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A438" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="B438" s="4" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="439" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A439" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="B439" s="4" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="440" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A440" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="B440" s="4" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="441" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A441" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="B441" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="442" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A442" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="B442" s="4" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="443" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A443" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="B443" s="4" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="444" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A444" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="B444" s="4" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="445" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A445" s="5" t="s">
+        <v>450</v>
+      </c>
+      <c r="B445" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="446" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A446" s="5" t="s">
+        <v>451</v>
+      </c>
+      <c r="B446" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="447" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A447" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="B447" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="448" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A448" s="5" t="s">
+        <v>453</v>
+      </c>
+      <c r="B448" s="4" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="505" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B505" s="5"/>
+    </row>
+    <row r="506" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B506" s="5"/>
+    </row>
+    <row r="507" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B507" s="5"/>
+    </row>
+    <row r="508" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B508" s="5"/>
+    </row>
+    <row r="509" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B509" s="5"/>
+    </row>
+    <row r="510" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B510" s="5"/>
+    </row>
+    <row r="511" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B511" s="5"/>
+    </row>
+    <row r="512" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B512" s="5"/>
+    </row>
+    <row r="513" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B513" s="5"/>
+    </row>
+    <row r="514" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B514" s="5"/>
+    </row>
+    <row r="515" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B515" s="5"/>
+    </row>
+    <row r="516" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B516" s="5"/>
+    </row>
+    <row r="517" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B517" s="5"/>
+    </row>
+    <row r="518" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B518" s="5"/>
+    </row>
+    <row r="519" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B519" s="5"/>
+    </row>
+    <row r="520" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B520" s="5"/>
+    </row>
+    <row r="521" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B521" s="5"/>
+    </row>
+    <row r="522" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B522" s="5"/>
+    </row>
+    <row r="523" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B523" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
updated the category file again
</commit_message>
<xml_diff>
--- a/event_category.xlsx
+++ b/event_category.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="180" windowWidth="27795" windowHeight="12525"/>
+    <workbookView xWindow="480" yWindow="240" windowWidth="27795" windowHeight="12465"/>
   </bookViews>
   <sheets>
     <sheet name="event_category" sheetId="1" r:id="rId1"/>
@@ -1762,8 +1762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B523"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A437" workbookViewId="0">
+      <selection activeCell="A452" sqref="A452"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>